<commit_message>
Update: Endentscheidungen zu Taggingfragen
Notebook: Visualisierung von DHA-Zotero (als Subdatenset) hinzugefügt
Filter_Varianten: Update
</commit_message>
<xml_diff>
--- a/keywords-inter-annotator-agreement/Filter_Varianten.xlsx
+++ b/keywords-inter-annotator-agreement/Filter_Varianten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43650\Documents\GitHub\vocabs-keywords\keywords-inter-annotator-agreement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B19F405-C87B-4E61-9A25-D37020488E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F1A5F6-08EB-437E-9985-08771E7D92A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D32BAA7B-F10D-428F-9617-76DBCF505210}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D32BAA7B-F10D-428F-9617-76DBCF505210}"/>
   </bookViews>
   <sheets>
     <sheet name="variants collection_dha_zenodo" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="3891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4056" uniqueCount="3894">
   <si>
     <t>Fremdsprachliche Tags (nicht dt oder engl)</t>
   </si>
@@ -11713,6 +11713,15 @@
   </si>
   <si>
     <t>sheet music</t>
+  </si>
+  <si>
+    <t>language arts &amp; disciplines</t>
+  </si>
+  <si>
+    <t>european</t>
+  </si>
+  <si>
+    <t>african american studies</t>
   </si>
 </sst>
 </file>
@@ -11762,11 +11771,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -12083,8 +12091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832D5A13-8A84-485F-937F-51CD76535623}">
   <dimension ref="A1:C1211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1154" workbookViewId="0">
-      <selection activeCell="B1202" sqref="B1202"/>
+    <sheetView topLeftCell="A1192" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17142,7 +17150,7 @@
       </c>
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B930" s="3" t="s">
+      <c r="B930" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -18737,8 +18745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F37E9-69CD-4C75-AF9B-16BA81871129}">
   <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19225,8 +19233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA7B861-B6D3-4585-B9F7-920F14327752}">
   <dimension ref="J1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19353,10 +19361,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7702E09-5076-489B-A602-06E3BA2397B3}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19364,7 +19372,7 @@
     <col min="1" max="1" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1534</v>
       </c>
@@ -19384,7 +19392,7 @@
         <v>3877</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -19398,7 +19406,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>254</v>
       </c>
@@ -19409,7 +19417,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>255</v>
       </c>
@@ -19420,7 +19428,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>256</v>
       </c>
@@ -19431,7 +19439,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -19442,7 +19450,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -19456,23 +19464,29 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>293</v>
       </c>
       <c r="B8" t="s">
         <v>1543</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="C8" t="s">
+        <v>3891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>294</v>
       </c>
       <c r="B9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>3891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>298</v>
       </c>
@@ -19483,15 +19497,30 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>299</v>
       </c>
       <c r="B11" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>3892</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3749</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>511</v>
       </c>
@@ -19502,7 +19531,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>540</v>
       </c>
@@ -19513,7 +19542,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>568</v>
       </c>
@@ -19524,7 +19553,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>607</v>
       </c>
@@ -19535,7 +19564,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>608</v>
       </c>
@@ -19711,6 +19740,15 @@
       <c r="A33" t="s">
         <v>997</v>
       </c>
+      <c r="B33" t="s">
+        <v>387</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2541</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3893</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -20124,7 +20162,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+      <c r="A79" t="s">
         <v>1413</v>
       </c>
       <c r="B79" t="s">
@@ -20138,7 +20176,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
+      <c r="A80" t="s">
         <v>861</v>
       </c>
       <c r="B80" t="s">
@@ -20579,7 +20617,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
+      <c r="A119" t="s">
         <v>858</v>
       </c>
       <c r="B119" t="s">

</xml_diff>